<commit_message>
update test for number input of LONIC and SNOMED code
</commit_message>
<xml_diff>
--- a/gamebus.xlsx
+++ b/gamebus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clgeng/github/strap/excel-to-fhir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE414D5-E6D9-0740-BF05-E63EBEE91283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F13F37-3598-4148-9231-88F8FB9B488A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{19EE9356-4A1B-BC4B-9204-784E3119BE99}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{19EE9356-4A1B-BC4B-9204-784E3119BE99}"/>
   </bookViews>
   <sheets>
     <sheet name="descriptor" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="101">
   <si>
     <t>type</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>WALK_L</t>
-  </si>
-  <si>
-    <t>S001</t>
   </si>
   <si>
     <t>WALK_S</t>
@@ -493,9 +490,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -533,7 +530,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -639,7 +636,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -781,7 +778,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -792,7 +789,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -814,7 +811,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -835,7 +832,7 @@
         <v>12</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>13</v>
@@ -844,7 +841,7 @@
         <v>14</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>15</v>
@@ -870,40 +867,40 @@
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="7">
+        <v>100</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>21</v>
-      </c>
       <c r="K2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -917,40 +914,40 @@
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -964,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>7</v>
@@ -972,24 +969,24 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1003,28 +1000,28 @@
         <v>0</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="K5" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -1033,37 +1030,37 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="J6" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -1097,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F1FA94-CD3A-C24A-831B-8E66C0BEE85F}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="256" zoomScaleNormal="256" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="180" zoomScaleNormal="256" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1112,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>4</v>
@@ -1124,7 +1121,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>13</v>
@@ -1133,76 +1130,76 @@
         <v>14</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>67</v>
+      </c>
+      <c r="B2" s="3">
+        <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="3">
+        <v>100</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1237,87 +1234,87 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1354,23 +1351,23 @@
   <sheetData>
     <row r="1" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1378,55 +1375,55 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -1434,7 +1431,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>